<commit_message>
Mejorando la claridad de los codigos
</commit_message>
<xml_diff>
--- a/codigo/vigas/ejemplos/viga_con_resortes.xlsx
+++ b/codigo/vigas/ejemplos/viga_con_resortes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="xnod" sheetId="1" state="visible" r:id="rId2"/>
@@ -34,7 +34,7 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author/>
+    <author> </author>
   </authors>
   <commentList>
     <comment ref="B1" authorId="0">
@@ -58,7 +58,7 @@
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author/>
+    <author> </author>
   </authors>
   <commentList>
     <comment ref="D1" authorId="0">
@@ -152,7 +152,7 @@
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author/>
+    <author> </author>
   </authors>
   <commentList>
     <comment ref="C1" authorId="0">
@@ -176,7 +176,7 @@
 <file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author/>
+    <author> </author>
   </authors>
   <commentList>
     <comment ref="C1" authorId="0">
@@ -200,7 +200,7 @@
 <file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author/>
+    <author> </author>
   </authors>
   <commentList>
     <comment ref="C1" authorId="0">
@@ -222,15 +222,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="29">
   <si>
     <t xml:space="preserve">nodo</t>
   </si>
   <si>
     <t xml:space="preserve">x</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Viga analizada en el Ejemplo 5-5 de Uribe Escamilla</t>
   </si>
   <si>
     <t xml:space="preserve">Unidades en kN y m</t>
@@ -449,12 +446,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -466,13 +463,13 @@
       <xdr:col>2</xdr:col>
       <xdr:colOff>375840</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>66960</xdr:rowOff>
+      <xdr:rowOff>72360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>54720</xdr:colOff>
+      <xdr:colOff>54360</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>110880</xdr:rowOff>
+      <xdr:rowOff>116280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -486,7 +483,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1582200" y="1333440"/>
-          <a:ext cx="6917760" cy="2034720"/>
+          <a:ext cx="6917400" cy="2034360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -508,14 +505,11 @@
   </sheetPr>
   <dimension ref="A1:D62"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D23" activeCellId="0" sqref="D23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.55102040816327"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -549,15 +543,12 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="n">
         <v>0.3</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -568,7 +559,7 @@
         <v>0.4</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1022,7 +1013,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1039,48 +1030,45 @@
   </sheetPr>
   <dimension ref="A1:M61"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="L3" activeCellId="0" sqref="L3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="8.55102040816327"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.3418367346939"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.23469387755102"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.719387755102"/>
-    <col collapsed="false" hidden="false" max="11" min="7" style="0" width="8.55102040816327"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="9.23469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="8.55102040816327"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="9.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="9.23"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1110,13 +1098,13 @@
         <v>0.025</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="L2" s="0" t="n">
         <v>0.1</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1146,13 +1134,13 @@
         <v>0.025</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L3" s="0" t="n">
         <v>0.3</v>
       </c>
       <c r="M3" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1182,13 +1170,13 @@
         <v>0.025</v>
       </c>
       <c r="K4" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="L4" s="3" t="n">
+        <v>210000000</v>
+      </c>
+      <c r="M4" s="0" t="s">
         <v>16</v>
-      </c>
-      <c r="L4" s="3" t="n">
-        <v>210000000</v>
-      </c>
-      <c r="M4" s="0" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1218,7 +1206,7 @@
         <v>0.025</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L5" s="0" t="n">
         <v>0.3</v>
@@ -1251,7 +1239,7 @@
         <v>0.025</v>
       </c>
       <c r="K6" s="0" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L6" s="0" t="n">
         <f aca="false">E/(2*(1+nu))</f>
@@ -1285,7 +1273,7 @@
         <v>0.025</v>
       </c>
       <c r="K7" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L7" s="0" t="n">
         <f aca="false">5/6</f>
@@ -1890,7 +1878,7 @@
         <v>-46</v>
       </c>
       <c r="K25" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2996,7 +2984,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3012,30 +3000,27 @@
   </sheetPr>
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I14" activeCellId="0" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.55102040816327"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>24</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3049,7 +3034,7 @@
         <v>0</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
@@ -3065,7 +3050,7 @@
         <v>0</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
@@ -3081,7 +3066,7 @@
         <v>0</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3095,13 +3080,13 @@
         <v>-0.05</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3117,15 +3102,15 @@
   </sheetPr>
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="4" width="8.55102040816327"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="4" width="14.75"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="4" width="8.55102040816327"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="4" width="8.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="4" width="14.75"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="4" style="4" width="8.55"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3133,22 +3118,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>24</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3164,31 +3149,28 @@
   </sheetPr>
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I14" activeCellId="0" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.55102040816327"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>28</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>29</v>
       </c>
       <c r="D1" s="4"/>
       <c r="E1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>24</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>25</v>
       </c>
       <c r="G1" s="4"/>
     </row>
@@ -3225,7 +3207,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>